<commit_message>
T110 - remove done
</commit_message>
<xml_diff>
--- a/venv/Data/try.xlsx
+++ b/venv/Data/try.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>是是是</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,19 +246,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>99g@snapmail.cc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>99g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>96f@snapmail.cc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>96f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98g@snapmail.cc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Passport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_CorpEmail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_CorpName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_DocumentType1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_DocumentType2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Rep1Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Rep1Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Rep2Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Rep2Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Rep3Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Rep3Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>National ID Card</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_Rep2Doc2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_NewProductName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99h@snapmail.cc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99hrep1@snapmail.cc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99hrep1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99hrep2@snapmail.cc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99hrep2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99hrep3@snapmail.cc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99hrep3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Link_NewCorp_WithRep_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -266,7 +362,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +407,12 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -333,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -345,6 +447,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -674,10 +777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -919,7 +1022,7 @@
         <v>51</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -935,7 +1038,7 @@
         <v>53</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -951,7 +1054,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -967,7 +1070,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -976,6 +1079,110 @@
       </c>
       <c r="B41" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1002,9 +1209,14 @@
     <hyperlink ref="B39" r:id="rId19"/>
     <hyperlink ref="B38" r:id="rId20"/>
     <hyperlink ref="B40" r:id="rId21" display="95d@snapmail.cc"/>
+    <hyperlink ref="B44" r:id="rId22"/>
+    <hyperlink ref="B46" r:id="rId23"/>
+    <hyperlink ref="B48" r:id="rId24"/>
+    <hyperlink ref="B52" r:id="rId25"/>
+    <hyperlink ref="B55" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
T110 competed new product
</commit_message>
<xml_diff>
--- a/venv/Data/try.xlsx
+++ b/venv/Data/try.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestEnv" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
   <si>
     <t>是是是</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -355,6 +355,10 @@
   </si>
   <si>
     <t>99h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T110_UploadDocument</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -777,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1183,6 +1187,14 @@
       </c>
       <c r="B56" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>